<commit_message>
Add `course-work` in `operation-research`
</commit_message>
<xml_diff>
--- a/3-course-6-semester/econometrics/task-10/task-10.xlsx
+++ b/3-course-6-semester/econometrics/task-10/task-10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mag\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bronn\Documents\github\university\3-course-6-semester\econometrics\task-10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56DBFF9-862D-492D-85FE-9B2A99F161A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB32691C-90AF-4B31-8F30-EF7E7C2D84D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{84367A3C-4C66-4C19-BD65-335C693477BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{84367A3C-4C66-4C19-BD65-335C693477BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,27 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
     <sheet name="Лист4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="57">
   <si>
     <t>Случайная компонента</t>
   </si>
@@ -193,6 +203,12 @@
   </si>
   <si>
     <t>F = 5,09</t>
+  </si>
+  <si>
+    <t>1 порядка</t>
+  </si>
+  <si>
+    <t>2 порядка</t>
   </si>
 </sst>
 </file>
@@ -200,7 +216,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -221,15 +237,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -257,11 +285,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -280,7 +323,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -338,7 +387,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -429,7 +478,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="ru-RU"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -479,7 +528,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="ru-RU"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -529,7 +578,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="ru-RU"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -579,7 +628,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="ru-RU"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -747,7 +796,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="613755352"/>
@@ -809,7 +858,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="613757648"/>
@@ -857,7 +906,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1623,14 +1672,26 @@
         </a:p>
         <a:p>
           <a:r>
+            <a:rPr lang="ru-RU" sz="1100" b="0" baseline="0"/>
+            <a:t>38</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>1.027</a:t>
+            <a:t>/37 = 1.027</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0"/>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" b="0" u="sng" baseline="0"/>
+            <a:t>Компоненты</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="sng" baseline="0"/>
+            <a:t>: </a:t>
+          </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
             <a:t>38 = 31 * 1.194 * 1.027</a:t>
@@ -2487,8 +2548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00B7F11C-1EB3-4281-B7FD-E0534B94366A}">
   <dimension ref="A8:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2524,216 +2585,200 @@
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
+      <c r="B38" s="9"/>
+      <c r="C38" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39">
+      <c r="B39" s="9">
         <v>1</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="9">
         <v>0</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40">
+      <c r="B40" s="9">
         <v>2</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="9">
         <v>3.2</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="9">
         <f t="shared" ref="E40:E47" si="0">C40*D40</f>
         <v>7.0400000000000009</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41">
+      <c r="B41" s="9">
         <v>3</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="9">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="9">
         <v>3.2</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="9">
         <f t="shared" si="0"/>
         <v>14.080000000000002</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="9">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42">
+      <c r="B42" s="9">
         <v>4</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="9">
         <v>5.5</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="9">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="9">
         <f t="shared" si="0"/>
         <v>24.200000000000003</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="9">
         <v>3.2</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43">
+      <c r="B43" s="9">
         <v>5</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="9">
         <v>6.7</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="9">
         <v>5.5</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="9">
         <f t="shared" si="0"/>
         <v>36.85</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="9">
         <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44">
+      <c r="B44" s="9">
         <v>6</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="9">
         <v>8.6</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="9">
         <v>6.7</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="9">
         <f t="shared" si="0"/>
         <v>57.62</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="9">
         <v>5.5</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45">
+      <c r="B45" s="9">
         <v>7</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="9">
         <v>10.6</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="9">
         <v>8.6</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="9">
         <f t="shared" si="0"/>
         <v>91.16</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="9">
         <v>6.7</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46">
+      <c r="B46" s="9">
         <v>8</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="9">
         <v>13.6</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="9">
         <v>10.6</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="9">
         <f t="shared" si="0"/>
         <v>144.16</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="9">
         <v>8.6</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47">
+      <c r="B47" s="9">
         <v>9</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="9">
         <v>17.3</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="9">
         <v>13.6</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="9">
         <f t="shared" si="0"/>
         <v>235.28</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="9">
         <v>10.6</v>
       </c>
     </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C50">
-        <f>AVERAGE(C39:C47)</f>
-        <v>8.0111111111111128</v>
-      </c>
-      <c r="D50">
-        <f>AVERAGE(D40:D47)</f>
-        <v>6.8500000000000005</v>
-      </c>
-      <c r="E50">
-        <f>AVERAGE(E39:E48)</f>
-        <v>67.821111111111108</v>
-      </c>
-    </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C51">
-        <f>VARPA(C39:C47)</f>
-        <v>22.505432098765404</v>
-      </c>
-      <c r="D51">
-        <f>VARPA(D40:D47)</f>
-        <v>13.184999999999988</v>
-      </c>
-    </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D53">
-        <v>1</v>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>55</v>
       </c>
       <c r="E53">
         <f>CORREL(C40:C47,D40:D47)</f>
         <v>0.99868339333424672</v>
       </c>
     </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D54">
-        <v>2</v>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>56</v>
       </c>
       <c r="E54">
         <f>CORREL(C41:C47,F41:F47)</f>
@@ -2750,8 +2795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E47A37E-8CD1-49DA-B7EC-7F764D093E0B}">
   <dimension ref="A7:Q120"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="P116" sqref="P116"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2760,175 +2805,175 @@
   </cols>
   <sheetData>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="11">
         <f>1/C8</f>
         <v>1.1627906976744186E-2</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="11">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="12">
         <v>86</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="12">
         <f>1/B8</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="11">
         <f t="shared" ref="A9:A17" si="0">1/C9</f>
         <v>1.5151515151515152E-2</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="11">
         <v>2</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="12">
         <v>66</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="12">
         <f t="shared" ref="D9:D17" si="1">1/B9</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="11">
         <f t="shared" si="0"/>
         <v>1.7241379310344827E-2</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="11">
         <v>3</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="12">
         <v>58</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="12">
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="11">
         <f t="shared" si="0"/>
         <v>1.8518518518518517E-2</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="11">
         <v>4</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="12">
         <v>54</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="12">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="11">
         <f t="shared" si="0"/>
         <v>1.9607843137254902E-2</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="11">
         <v>5</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="12">
         <v>51</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="12">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="11">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="11">
         <v>6</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="12">
         <v>50</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="12">
         <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="11">
         <f t="shared" si="0"/>
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="11">
         <v>7</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="12">
         <v>48</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="12">
         <f t="shared" si="1"/>
         <v>0.14285714285714285</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="11">
         <f t="shared" si="0"/>
         <v>2.1276595744680851E-2</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="11">
         <v>8</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="12">
         <v>47</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="12">
         <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="11">
         <f t="shared" si="0"/>
         <v>2.1739130434782608E-2</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="11">
         <v>9</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="12">
         <v>46</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="12">
         <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="11">
         <f t="shared" si="0"/>
         <v>2.1739130434782608E-2</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="11">
         <v>10</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="12">
         <v>46</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="12">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
@@ -3749,7 +3794,7 @@
         <v>6.2361785648404338</v>
       </c>
       <c r="N107">
-        <f t="shared" ref="N107:N116" si="2">K107^2</f>
+        <f t="shared" ref="N107:N115" si="2">K107^2</f>
         <v>2.1948504332544232</v>
       </c>
     </row>
@@ -3767,7 +3812,7 @@
         <v>1.4815027618112708</v>
       </c>
       <c r="M108">
-        <f t="shared" ref="M108:M116" si="3">(K108-L108)^2</f>
+        <f t="shared" ref="M108:M115" si="3">(K108-L108)^2</f>
         <v>0.25092278896506448</v>
       </c>
       <c r="N108">
@@ -4628,7 +4673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7215CF-4BF9-416E-8C29-0907953235D5}">
   <dimension ref="D4:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>